<commit_message>
Report, scatter plot scripts, updated README, added cases 33,34,35 results
</commit_message>
<xml_diff>
--- a/PowerVariabilityScenarios.xlsx
+++ b/PowerVariabilityScenarios.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/rshashikumar_wisc_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/rshashikumar_wisc_edu/Documents/Rajesh/git/mlsys-gpu-power-variability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="372" documentId="8_{9EFFBDD1-998F-4EDC-AF64-BC711F7C86A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BB233B1-54EB-4C7B-A910-85A525D7911F}"/>
+  <xr:revisionPtr revIDLastSave="378" documentId="8_{9EFFBDD1-998F-4EDC-AF64-BC711F7C86A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5E025BD-EC38-4344-98FB-16AF0F62AD3B}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{3E3D7084-F92D-48A1-8897-57E0DB02C5B5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Scenarios" sheetId="4" r:id="rId1"/>
+    <sheet name="Old" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="74">
   <si>
     <t>GPU1</t>
   </si>
@@ -272,6 +272,42 @@
   <si>
     <t>a</t>
   </si>
+  <si>
+    <t>Effect of increasing number of GPUs on noise workloads</t>
+  </si>
+  <si>
+    <t>9 (4)</t>
+  </si>
+  <si>
+    <t>Effect of homogenous workload on each other (Time locality)</t>
+  </si>
+  <si>
+    <t>Spatial effects (3): Does GPU allocation in a cluster impact performance?</t>
+  </si>
+  <si>
+    <t>Effect of distributed training on base</t>
+  </si>
+  <si>
+    <t>Effect of data movement on base</t>
+  </si>
+  <si>
+    <t>Manually choose best GPU in terms of idle temp to see if it performs better?</t>
+  </si>
+  <si>
+    <t>Effect of heterogeneous utilization on base workload</t>
+  </si>
+  <si>
+    <t>Proving that temperature effect due to spatial proximity affects performance (runtimetime/frequency)</t>
+  </si>
+  <si>
+    <t>case33</t>
+  </si>
+  <si>
+    <t>case34</t>
+  </si>
+  <si>
+    <t>case35</t>
+  </si>
 </sst>
 </file>
 
@@ -294,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +370,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -512,6 +554,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -527,12 +587,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,11 +596,41 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,11 +945,852 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A93E3A4-139A-4785-B217-7F151AFE5C35}">
+  <dimension ref="A1:J38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.23046875" style="48" customWidth="1"/>
+    <col min="3" max="3" width="9.23046875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.84375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.53515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.4609375" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="3.3046875" customWidth="1"/>
+    <col min="9" max="9" width="10.07421875" customWidth="1"/>
+    <col min="10" max="10" width="8.07421875" customWidth="1"/>
+    <col min="11" max="11" width="12.07421875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" s="38">
+        <v>1</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" s="38">
+        <v>2</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="38">
+        <v>3</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" s="38">
+        <v>4</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" s="38">
+        <v>5</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" s="38">
+        <v>6</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" s="38">
+        <v>7</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" s="38">
+        <v>8</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A10" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" s="38">
+        <v>10</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12" s="38">
+        <v>11</v>
+      </c>
+      <c r="B12" s="41"/>
+      <c r="C12" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13" s="38">
+        <v>12</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14" s="38">
+        <v>13</v>
+      </c>
+      <c r="B14" s="41"/>
+      <c r="C14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15" s="38">
+        <v>14</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16" s="38">
+        <v>15</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" s="38">
+        <v>16</v>
+      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" s="38">
+        <v>17</v>
+      </c>
+      <c r="B18" s="44"/>
+      <c r="C18" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19" s="38">
+        <v>18</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" s="38">
+        <v>20</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21" s="38">
+        <v>21</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22" s="38">
+        <v>22</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A23" s="38">
+        <v>23</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A24" s="38">
+        <v>24</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25" s="38">
+        <v>25</v>
+      </c>
+      <c r="B25" s="41"/>
+      <c r="C25" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26" s="38">
+        <v>26</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27" s="38">
+        <v>27</v>
+      </c>
+      <c r="B27" s="41"/>
+      <c r="C27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="25"/>
+      <c r="G27" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28" s="38">
+        <v>28</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="25"/>
+      <c r="G28" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A29" s="38">
+        <v>29</v>
+      </c>
+      <c r="B29" s="41"/>
+      <c r="C29" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="25"/>
+      <c r="E29" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30" s="38">
+        <v>30</v>
+      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31" s="38">
+        <v>19</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32" s="38">
+        <v>31</v>
+      </c>
+      <c r="B32" s="46"/>
+      <c r="C32" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="14.6" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="38">
+        <v>32</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A34" s="38">
+        <v>32</v>
+      </c>
+      <c r="B34" s="47"/>
+      <c r="C34" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="25"/>
+      <c r="F34" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A35" s="38">
+        <v>33</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A36" s="38">
+        <v>34</v>
+      </c>
+      <c r="B36" s="39"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A37" s="38">
+        <v>35</v>
+      </c>
+      <c r="B37" s="39"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="D19:F19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA65C5A-F3A0-44E1-98CB-05931604F659}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -907,7 +1832,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="27" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -927,7 +1852,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="11" t="s">
         <v>3</v>
       </c>
@@ -947,7 +1872,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
@@ -969,7 +1894,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="34"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="11" t="s">
         <v>3</v>
       </c>
@@ -1141,7 +2066,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -1167,7 +2092,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
@@ -1223,7 +2148,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="26" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -1252,7 +2177,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="13" t="s">
         <v>5</v>
       </c>
@@ -1273,7 +2198,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="13" t="s">
         <v>5</v>
       </c>
@@ -1300,11 +2225,11 @@
       <c r="C19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
+      <c r="D19" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
       <c r="G19" s="1" t="s">
         <v>43</v>
       </c>
@@ -1322,10 +2247,10 @@
       <c r="D20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="24"/>
+      <c r="E20" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="30"/>
       <c r="G20" s="1" t="s">
         <v>44</v>
       </c>
@@ -1334,7 +2259,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -1360,7 +2285,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="26"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="11" t="s">
         <v>3</v>
       </c>
@@ -1381,7 +2306,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="27"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="11" t="s">
         <v>3</v>
       </c>
@@ -1463,7 +2388,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -1486,17 +2411,17 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="29"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="31"/>
+      <c r="E28" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="35"/>
       <c r="G28" s="1" t="s">
         <v>49</v>
       </c>
@@ -1505,7 +2430,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="26" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -1514,10 +2439,10 @@
       <c r="D29" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="31"/>
+      <c r="E29" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="35"/>
       <c r="G29" s="1" t="s">
         <v>50</v>
       </c>
@@ -1526,11 +2451,11 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="32"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="36"/>
       <c r="E30" s="11" t="s">
         <v>3</v>
       </c>
@@ -1545,12 +2470,12 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="35"/>
+      <c r="E31" s="36"/>
       <c r="F31" s="11" t="s">
         <v>3</v>
       </c>
@@ -1565,10 +2490,10 @@
       <c r="B32" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="24"/>
+      <c r="C32" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="30"/>
       <c r="E32" s="11" t="s">
         <v>3</v>
       </c>
@@ -1607,12 +2532,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B16:B18"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="B21:B23"/>
@@ -1623,432 +2542,14 @@
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:E31"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B16:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE926DE3-FC85-4D11-B8CF-353E7D1E1E44}">
-  <dimension ref="C1:F32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C5" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C6" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C9" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C11" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C12" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C13" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C14" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C15" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C16" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C17" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C19" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="24"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C20" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C21" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C22" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C23" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C25" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C26" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C27" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" s="31"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C28" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="31"/>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C29" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="32"/>
-      <c r="E29" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C30" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="31"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C31" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C32" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:E30"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>